<commit_message>
added tablesaw code to get value from almost any type of input data or file including resultset, attempt somewhat use benefits of dataframe using table
</commit_message>
<xml_diff>
--- a/test_data/driver_excel.xlsx
+++ b/test_data/driver_excel.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\java_practice\framework_build_project\test_dev_project\Testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\java_practice\framework_build_project\test_dev_project\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2FDEA4-F111-401E-B573-8D273FD465B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2B8DB8-7699-45CC-9E23-0B49F8B1E412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="test_sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="test_sheet_1" sheetId="1" r:id="rId1"/>
+    <sheet name="test_sheet_2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>test_keyword</t>
   </si>
@@ -67,6 +68,12 @@
   </si>
   <si>
     <t>Intel Pentium Dual Core</t>
+  </si>
+  <si>
+    <t>test_1_2</t>
+  </si>
+  <si>
+    <t>test_2_2</t>
   </si>
 </sst>
 </file>
@@ -386,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,4 +458,77 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F22B05A1-6698-4D23-8004-A4AFE2154C9F}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>